<commit_message>
update intro y tablas
</commit_message>
<xml_diff>
--- a/input/tables/table-1.xlsx
+++ b/input/tables/table-1.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julio\Dropbox\papers\padsoc\input\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB64F2C-7106-4707-90C0-FC9C2F51D335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EA4327-714F-4AD9-A0FD-38B642056D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t xml:space="preserve">(a) preprueba/postprueba, (b) sólo postprueba, (c) postpruebas múltiples, (d) roll-out, (e) crossover, (f) Salomón de cuatro grupos, (g) factorial. </t>
   </si>
@@ -46,6 +47,57 @@
   </si>
   <si>
     <t xml:space="preserve">3. Más allá de X e Y (factores distintos de la covariación de X e Y) </t>
+  </si>
+  <si>
+    <t>Modalidad</t>
+  </si>
+  <si>
+    <t>Presencial</t>
+  </si>
+  <si>
+    <t>Autoadministrado</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>Administración</t>
+  </si>
+  <si>
+    <t>Entidad externa (p.ej. Consultora)</t>
+  </si>
+  <si>
+    <t>Plataforma web (p.ej. Qualtrics)</t>
+  </si>
+  <si>
+    <t>Mediado por</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>`.csv`, `.sav`</t>
+  </si>
+  <si>
+    <t>Libro de códigos</t>
+  </si>
+  <si>
+    <t>Formato de datos</t>
+  </si>
+  <si>
+    <t>Cara a cara (*CAPI*)</t>
+  </si>
+  <si>
+    <t>\-</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\- </t>
+  </si>
+  <si>
+    <t>Etiquetado variables</t>
   </si>
 </sst>
 </file>
@@ -368,7 +420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -416,4 +468,87 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7ED05F3-0E05-4EF3-A004-0EA8F52DCB2D}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>